<commit_message>
Add More API and Modify
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="19440" windowHeight="12600" tabRatio="986" firstSheet="8" activeTab="14"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="19440" windowHeight="12600" tabRatio="986" firstSheet="12" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Banner" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="CopyRight" sheetId="14" r:id="rId16"/>
     <sheet name="HelpCenter" sheetId="15" r:id="rId17"/>
     <sheet name="Dynamic" sheetId="16" r:id="rId18"/>
-    <sheet name="Industry_Info" sheetId="17" r:id="rId19"/>
+    <sheet name="Industry" sheetId="17" r:id="rId19"/>
     <sheet name="Recruitment" sheetId="18" r:id="rId20"/>
     <sheet name="Guide" sheetId="19" r:id="rId21"/>
     <sheet name="Product" sheetId="20" r:id="rId22"/>
@@ -210,12 +210,6 @@
     <t>Position</t>
   </si>
   <si>
-    <t>Address_Information</t>
-  </si>
-  <si>
-    <t>Address_Picture</t>
-  </si>
-  <si>
     <t>Copyright_Title</t>
   </si>
   <si>
@@ -237,51 +231,18 @@
     <t>Dynamic_Content</t>
   </si>
   <si>
-    <t>Headline</t>
-  </si>
-  <si>
-    <t>Info_Subtitle</t>
-  </si>
-  <si>
-    <t>Info_Img</t>
-  </si>
-  <si>
-    <t>Info_Content</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
-    <t>Boot_Page_Title</t>
-  </si>
-  <si>
-    <t>Boot_Page_Img</t>
-  </si>
-  <si>
     <t>Product_Title</t>
   </si>
   <si>
-    <t>Cover_Map</t>
-  </si>
-  <si>
-    <t>Promotion</t>
-  </si>
-  <si>
-    <t>Original_Price</t>
-  </si>
-  <si>
     <t>Double</t>
   </si>
   <si>
     <t>Start_Price</t>
   </si>
   <si>
-    <t>Commodity_Booking</t>
-  </si>
-  <si>
-    <t>Associated_Project</t>
-  </si>
-  <si>
     <t>Price_Description</t>
   </si>
   <si>
@@ -420,9 +381,6 @@
     <t>QA_Id</t>
   </si>
   <si>
-    <t>Product_Project</t>
-  </si>
-  <si>
     <t>Product_Id</t>
   </si>
   <si>
@@ -487,6 +445,48 @@
   </si>
   <si>
     <t>Member_Img</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>Contact_Img</t>
+  </si>
+  <si>
+    <t>Industry_Title</t>
+  </si>
+  <si>
+    <t>Industry_Subtitle</t>
+  </si>
+  <si>
+    <t>Industry_Img</t>
+  </si>
+  <si>
+    <t>Industry_Content</t>
+  </si>
+  <si>
+    <t>BootPage_Title</t>
+  </si>
+  <si>
+    <t>BootPage_Img</t>
+  </si>
+  <si>
+    <t>Cover_Img</t>
+  </si>
+  <si>
+    <t>Promotion_Img</t>
+  </si>
+  <si>
+    <t>Promotion_Image</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>Origin_Price</t>
+  </si>
+  <si>
+    <t>Booking</t>
   </si>
 </sst>
 </file>
@@ -835,25 +835,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="1504950" y="1333500"/>
-          <a:ext cx="2038350" cy="390525"/>
+        <a:xfrm>
+          <a:off x="1866900" y="876300"/>
+          <a:ext cx="1676400" cy="942975"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1313,7 +1313,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1330,10 +1330,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="D5" s="3"/>
     </row>
@@ -1354,7 +1354,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1379,7 +1379,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1409,31 +1409,31 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -1441,21 +1441,21 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>2</v>
@@ -1466,13 +1466,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>13</v>
@@ -1480,13 +1480,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>10</v>
@@ -1500,7 +1500,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>10</v>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="E12" s="6" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>10</v>
@@ -1520,13 +1520,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>10</v>
@@ -1571,15 +1571,15 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -1598,7 +1598,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1679,7 +1679,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>10</v>
@@ -1703,7 +1703,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>29</v>
@@ -1738,7 +1738,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1886,7 +1886,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>29</v>
@@ -1905,7 +1905,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1926,8 +1926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>56</v>
+        <v>135</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>57</v>
+        <v>136</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
@@ -2005,7 +2005,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>
@@ -2013,7 +2013,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
@@ -2079,7 +2079,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A7:B7"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
@@ -2122,7 +2122,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>29</v>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>29</v>
@@ -2157,7 +2157,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2179,12 +2179,12 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2206,7 +2206,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>65</v>
+        <v>137</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>
@@ -2214,7 +2214,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>66</v>
+        <v>138</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>29</v>
@@ -2230,7 +2230,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>29</v>
@@ -2257,7 +2257,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>
@@ -2318,7 +2318,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2326,7 +2326,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2352,7 +2352,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2378,7 +2378,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>
@@ -2414,7 +2414,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>
@@ -2450,7 +2450,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
@@ -2466,18 +2466,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2488,10 +2488,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2521,7 +2521,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>
@@ -2529,7 +2529,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
@@ -2537,37 +2537,35 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>29</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>75</v>
+        <v>147</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>78</v>
+        <v>148</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>2</v>
@@ -2578,11 +2576,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E9" s="6" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>13</v>
@@ -2590,13 +2590,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>10</v>
@@ -2604,44 +2604,48 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>95</v>
+        <v>146</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>10</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2681,7 +2685,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>
@@ -2689,7 +2693,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
@@ -2705,7 +2709,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>29</v>
@@ -2713,7 +2717,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>29</v>
@@ -2721,7 +2725,7 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>29</v>
@@ -2729,7 +2733,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>29</v>
@@ -2795,7 +2799,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
@@ -2803,7 +2807,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>29</v>
@@ -2819,7 +2823,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>29</v>
@@ -2827,22 +2831,22 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>2</v>
@@ -2853,13 +2857,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>10</v>
@@ -2867,10 +2871,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E11" s="6" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2912,7 +2916,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>
@@ -2987,7 +2991,7 @@
         <v>13</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -2998,41 +3002,41 @@
         <v>29</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -3043,26 +3047,26 @@
         <v>29</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>29</v>
@@ -3076,13 +3080,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>10</v>
@@ -3090,16 +3094,16 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3154,15 +3158,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
@@ -3173,7 +3177,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3181,7 +3185,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3231,7 +3235,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>10</v>
@@ -3239,7 +3243,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -3247,7 +3251,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>29</v>
@@ -3255,7 +3259,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>29</v>
@@ -3394,7 +3398,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -3447,7 +3451,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3455,7 +3459,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3553,10 +3557,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -3650,12 +3654,12 @@
         <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>
@@ -3669,7 +3673,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -3689,7 +3693,7 @@
         <v>29</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>10</v>
@@ -3703,7 +3707,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>10</v>
@@ -3717,7 +3721,7 @@
         <v>29</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>10</v>
@@ -3731,10 +3735,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>10</v>
@@ -3745,7 +3749,7 @@
         <v>40</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3822,10 +3826,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3833,10 +3837,10 @@
         <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3861,7 +3865,7 @@
         <v>29</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>10</v>
@@ -3875,7 +3879,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>10</v>
@@ -3889,7 +3893,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>10</v>
@@ -3903,7 +3907,7 @@
         <v>29</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>10</v>
@@ -3917,7 +3921,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>10</v>
@@ -3928,10 +3932,10 @@
         <v>48</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="F11" s="7"/>
     </row>
@@ -3940,7 +3944,7 @@
         <v>49</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>2</v>
@@ -3957,7 +3961,7 @@
         <v>29</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>10</v>
@@ -3971,7 +3975,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>10</v>
@@ -3985,7 +3989,7 @@
         <v>29</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>10</v>
@@ -4015,7 +4019,7 @@
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" s="6" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>10</v>
@@ -4023,7 +4027,7 @@
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20" s="6" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>10</v>
@@ -4031,10 +4035,10 @@
     </row>
     <row r="21" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E21" s="6" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -4080,7 +4084,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>10</v>
@@ -4088,10 +4092,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4106,7 +4110,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>29</v>
@@ -4116,13 +4120,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>